<commit_message>
update bang tong hop nhan su
</commit_message>
<xml_diff>
--- a/ASP.NET CORE/HRMNS/HRMS/wwwroot/templates/RegisterTimeKeepingTemplate.xlsx
+++ b/ASP.NET CORE/HRMNS/HRMS/wwwroot/templates/RegisterTimeKeepingTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>MaNV</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>BM : Làm ca đêm ngày kỷ niệm trước lễ chính thức</t>
-  </si>
-  <si>
-    <t>T : Nghỉ việc</t>
   </si>
   <si>
     <t>H2105001</t>
@@ -312,14 +309,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 70" xfId="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -608,8 +598,8 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,21 +622,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="13" t="s">
         <v>46</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -665,7 +655,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>KyTuChamCong!$A$1:$A$40</xm:f>
+            <xm:f>KyTuChamCong!$A$1:$A$39</xm:f>
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
@@ -680,10 +670,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,42 +1079,35 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
+        <v>38</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
     </row>
-    <row r="39" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
     </row>
-    <row r="40" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A37:A40">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="A36:A39">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>IF(A$16="sun",1,0)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update hrms and omns
</commit_message>
<xml_diff>
--- a/ASP.NET CORE/HRMNS/HRMS/wwwroot/templates/RegisterTimeKeepingTemplate.xlsx
+++ b/ASP.NET CORE/HRMNS/HRMS/wwwroot/templates/RegisterTimeKeepingTemplate.xlsx
@@ -15,7 +15,10 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="KyTuChamCong" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" calcOnSave="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$F$2</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>MaNV</t>
   </si>
@@ -177,7 +180,61 @@
     <t>T: Nghỉ việc</t>
   </si>
   <si>
-    <t>AL30</t>
+    <t>AL30:AL30</t>
+  </si>
+  <si>
+    <t>KR_1: Nghỉ phép năm</t>
+  </si>
+  <si>
+    <t>KR_2: Nghỉ nửa ngày</t>
+  </si>
+  <si>
+    <t>KR_3: Nghỉ 1/4 ngày</t>
+  </si>
+  <si>
+    <t>KR_4: Trực</t>
+  </si>
+  <si>
+    <t>KR_5: Tắc đường (đến muộn một chút)</t>
+  </si>
+  <si>
+    <t>KR_6: Nghỉ ốm (đi bệnh viện)</t>
+  </si>
+  <si>
+    <t>KR_7: Tiếp khách</t>
+  </si>
+  <si>
+    <t>KR_8: Công tác</t>
+  </si>
+  <si>
+    <t>KR_9: Thăm gia đình</t>
+  </si>
+  <si>
+    <t>KR_10: Đi muộn</t>
+  </si>
+  <si>
+    <t>KR_11: Đi làm đặc biệt</t>
+  </si>
+  <si>
+    <t>KR_12: Họp</t>
+  </si>
+  <si>
+    <t>KR_13: Thông ca</t>
+  </si>
+  <si>
+    <t>KR_14: Nghỉ lễ</t>
+  </si>
+  <si>
+    <t>KR_15: Ở nhà làm việc</t>
+  </si>
+  <si>
+    <t>KR_16: Không chấm công</t>
+  </si>
+  <si>
+    <t>KR_17: Nghỉ hiếu</t>
+  </si>
+  <si>
+    <t>L160:Nghỉ hưởng 160k</t>
   </si>
 </sst>
 </file>
@@ -220,7 +277,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +293,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,7 +344,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -316,19 +379,13 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 70" xfId="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -618,7 +675,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +731,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>KyTuChamCong!$A$1:$A$43</xm:f>
+            <xm:f>KyTuChamCong!$A$1:$A$61</xm:f>
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
@@ -689,10 +746,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,9 +1201,99 @@
         <v>50</v>
       </c>
     </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A36:A43">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="A36:A44">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>IF(A$16="sun",1,0)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>